<commit_message>
FeatureRM #380 (ci,tes): Add debug variant tests (*.json) and create 2 test name in order to:   . loop on all debug variant tests   . loop on all functional variant tests.
</commit_message>
<xml_diff>
--- a/simu/conf/fpasim/tes/tes_top_test_list.xlsx
+++ b/simu/conf/fpasim/tes/tes_top_test_list.xlsx
@@ -22,7 +22,7 @@
   </office:font-face-decls>
   <office:automatic-styles>
     <style:style style:name="co1" style:family="table-column">
-      <style:table-column-properties fo:break-before="auto" style:column-width="5.473cm"/>
+      <style:table-column-properties fo:break-before="auto" style:column-width="7.516cm"/>
     </style:style>
     <style:style style:name="co2" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="8.197cm"/>
@@ -31,6 +31,9 @@
       <style:table-column-properties fo:break-before="auto" style:column-width="6.371cm"/>
     </style:style>
     <style:style style:name="co4" style:family="table-column">
+      <style:table-column-properties fo:break-before="auto" style:column-width="8.495cm"/>
+    </style:style>
+    <style:style style:name="co5" style:family="table-column">
       <style:table-column-properties fo:break-before="auto" style:column-width="2.258cm"/>
     </style:style>
     <style:style style:name="ro1" style:family="table-row">
@@ -48,8 +51,9 @@
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
     </style:style>
-    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties fo:background-color="#00a933"/>
+    <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#00a933" style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
     </style:style>
     <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
@@ -62,9 +66,23 @@
     <style:style style:name="ce9" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#808080"/>
     </style:style>
-    <style:style style:name="ce3" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:vertical-align="middle"/>
+    <style:style style:name="ce12" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#eeeeee" style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #000000" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
+    </style:style>
+    <style:style style:name="ce13" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:border="0.06pt solid #000000" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
+    </style:style>
+    <style:style style:name="ce14" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#eeeeee" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" fo:border="0.06pt solid #000000" style:vertical-align="middle"/>
       <style:paragraph-properties fo:text-align="start" fo:margin-left="0cm"/>
+    </style:style>
+    <style:style style:name="ce15" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:border="0.06pt solid #000000"/>
+    </style:style>
+    <style:style style:name="ce16" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#eeeeee" fo:border="0.06pt solid #000000"/>
     </style:style>
     <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:vertical-align="top"/>
@@ -72,31 +90,60 @@
     <style:style style:name="ce11" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#808080" style:vertical-align="top"/>
     </style:style>
+    <style:style style:name="ce19" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#eeeeee" fo:border="0.06pt solid #000000" style:vertical-align="top"/>
+    </style:style>
+    <style:style style:name="ce20" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:border="0.06pt solid #000000" style:vertical-align="top"/>
+    </style:style>
+    <style:style style:name="ce21" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0cm"/>
+    </style:style>
     <style:style style:name="T1" style:family="text">
       <style:text-properties style:font-name="Liberation Sans" fo:font-size="10pt" fo:font-weight="normal" style:text-underline-style="none" style:text-underline-color="font-color" style:text-line-through-type="none" fo:font-style="normal" style:text-outline="false" fo:text-shadow="none" style:text-line-through-mode="continuous" fo:language="fr" fo:country="FR" style:language-asian="zh" style:country-asian="CN" style:language-complex="hi" style:country-complex="IN" style:font-name-asian="Microsoft YaHei" style:font-name-complex="Arial" style:font-size-asian="10pt" style:font-size-complex="10pt" style:font-weight-asian="normal" style:font-weight-complex="normal" style:font-style-asian="normal" style:font-style-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
+    <style:style style:name="T2" style:family="text">
+      <style:text-properties fo:color="#c9211e"/>
+    </style:style>
+    <style:style style:name="T3" style:family="text">
+      <style:text-properties fo:color="#000000"/>
+    </style:style>
+    <style:style style:name="T4" style:family="text">
+      <style:text-properties fo:color="#ff0000"/>
+    </style:style>
+    <style:style style:name="T5" style:family="text">
+      <style:text-properties style:font-name="Liberation Sans" fo:font-size="10pt" fo:font-weight="normal" style:text-underline-style="none" style:text-underline-color="font-color" style:text-line-through-type="none" fo:font-style="normal" style:text-outline="false" fo:text-shadow="none" style:text-line-through-mode="continuous" fo:language="fr" fo:country="FR" style:language-asian="zh" style:country-asian="CN" style:language-complex="hi" style:country-complex="IN" style:font-name-asian="Microsoft YaHei" style:font-name-complex="Arial" style:font-size-asian="10pt" style:font-size-complex="10pt" style:font-weight-asian="normal" style:font-weight-complex="normal" style:font-style-asian="normal" style:font-style-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color" fo:color="#c9211e"/>
+    </style:style>
+    <style:style style:name="T6" style:family="text">
+      <style:text-properties style:font-name="Liberation Sans" fo:font-size="10pt" fo:font-weight="normal" style:text-underline-style="none" style:text-underline-color="font-color" style:text-line-through-type="none" fo:font-style="normal" style:text-outline="false" fo:text-shadow="none" style:text-line-through-mode="continuous" fo:language="fr" fo:country="FR" style:language-asian="zh" style:country-asian="CN" style:language-complex="hi" style:country-complex="IN" style:font-name-asian="Microsoft YaHei" style:font-name-complex="Arial" style:font-size-asian="10pt" style:font-size-complex="10pt" style:font-weight-asian="normal" style:font-weight-complex="normal" style:font-style-asian="normal" style:font-style-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color" fo:color="#ff0000"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
     <office:spreadsheet>
       <table:table table:name="Feuille1" table:style-name="ta1">
-        <table:table-column table:style-name="co1" table:default-cell-style-name="ce2"/>
+        <table:table-column table:style-name="co1" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co3" table:default-cell-style-name="ce4"/>
-        <table:table-column table:style-name="co4" table:number-columns-repeated="1021" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co3" table:default-cell-style-name="Default"/>
+        <table:table-column table:style-name="co4" table:default-cell-style-name="ce2"/>
+        <table:table-column table:style-name="co5" table:number-columns-repeated="1020" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>test_name</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>parameters summary</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
+            <text:p>reading speed</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce5" office:value-type="string" calcext:value-type="string">
             <text:p>comment</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_func00.json</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -108,21 +155,24 @@
             <text:p>"pixel_id_list": [0],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              <text:span text:style-name="T1">Continuous reading</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
+            <text:p>Nominal case with different pixel_id</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_func01.json</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -134,21 +184,22 @@
             <text:p>"pixel_id_list": [16],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              <text:span text:style-name="T1">Continuous reading</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_func02.json</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -160,27 +211,29 @@
             <text:p>"pixel_id_list": [33],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              <text:span text:style-name="T1">Continuous reading</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce7"/>
           <table:table-cell table:style-name="ce9"/>
           <table:table-cell table:style-name="ce11"/>
-          <table:table-cell table:style-name="ce9" table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7"/>
+          <table:table-cell table:style-name="ce9" table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_func03.json</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -192,19 +245,24 @@
             <text:p>"pixel_id_list": [0],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Continuous reading</text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="3">
+            <text:p>High limit case with different pixel_id</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_func04.json</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -216,21 +274,22 @@
             <text:p>"pixel_id_list": [31],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              <text:span text:style-name="T1">Continuous reading</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_func05.json</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -242,27 +301,29 @@
             <text:p>"pixel_id_list": [63],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              <text:span text:style-name="T1">Continuous reading</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:covered-table-cell/>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro4">
           <table:table-cell table:style-name="ce7"/>
           <table:table-cell table:style-name="ce9"/>
           <table:table-cell table:style-name="ce11"/>
-          <table:table-cell table:style-name="ce9" table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7"/>
+          <table:table-cell table:style-name="ce9" table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_func06.json</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -274,27 +335,37 @@
             <text:p>"pixel_id_list": [0],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>
-              <text:span text:style-name="T1">Continuous reading</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce21" office:value-type="string" calcext:value-type="string">
+            <text:p>Low limit case </text:p>
+            <text:p/>
+            <text:p>
+              <text:span text:style-name="T2">Important</text:span>
+               : the user shouldn’t set a pixel_id different of 0.
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce9" table:number-columns-repeated="1024"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce9" table:number-columns-repeated="3"/>
+          <table:table-cell table:style-name="ce7"/>
+          <table:table-cell table:style-name="ce9" table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_debug00.json</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce14" office:value-type="string" calcext:value-type="string">
             <text:p>
               <text:span text:style-name="T1">"</text:span>
               nb_pixel_by_frame": 8
@@ -306,25 +377,27 @@
             <text:p>"pixel_id_list": [0],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Test small pulse (debug)</text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous data valid</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce19" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>small pulse</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_debug01.json</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>"nb_pixel_by_frame": 8,</text:p>
             <text:p>"nb_sample_by_pixel": 8,</text:p>
             <text:p>"nb_frame_by_pulse": 2048,</text:p>
@@ -333,25 +406,27 @@
             <text:p>"pixel_id_list": [0],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>test negative pulse (debug)</text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous data valid</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>pulse with output negative value (I0&lt;0)</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_debug02.json</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce16" office:value-type="string" calcext:value-type="string">
             <text:p>"nb_pixel_by_frame": 8,</text:p>
             <text:p>"nb_sample_by_pixel": 8,</text:p>
             <text:p>"nb_frame_by_pulse": 2048,</text:p>
@@ -360,25 +435,27 @@
             <text:p>"pixel_id_list": [0],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>test big pulse (debug)</text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous data valid</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce19" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>big pulse</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>tb_tes_top_test_variant_debug03.json</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>"nb_pixel_by_frame": 1,</text:p>
             <text:p>"nb_sample_by_pixel": 6,</text:p>
             <text:p>"nb_frame_by_pulse": 2048,</text:p>
@@ -387,19 +464,267 @@
             <text:p>"pixel_id_list": [0],</text:p>
             <text:p>"time_shift_list": [2],</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>test minimum samples by pixel</text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous data valid</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
-            </text:p>
-            <text:p>
-              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
-            </text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1021"/>
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>Lowest authorized number of samples of pixel</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>tb_tes_top_test_variant_debug04.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce14" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">"</text:span>
+              nb_pixel_by_frame": 8
+            </text:p>
+            <text:p>"nb_sample_by_pixel": 8,</text:p>
+            <text:p>"nb_frame_by_pulse": 2048,</text:p>
+            <text:p>"nb_pulse": 1,</text:p>
+            <text:p>"pulse_height_list": [16384],</text:p>
+            <text:p>"pixel_id_list": [0],</text:p>
+            <text:p>"time_shift_list": [2],</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce19" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T5">sporadic ram1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T5">sporadic ram2 check</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Sporadic RAM writting</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>tb_tes_top_test_variant_debug05.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>"nb_pixel_by_frame": 34,</text:p>
+            <text:p>"nb_sample_by_pixel": 8,</text:p>
+            <text:p>"nb_frame_by_pulse": 2048,</text:p>
+            <text:p>"nb_pulse": 1,</text:p>
+            <text:p>"pulse_height_list": [58880],</text:p>
+            <text:p>"pixel_id_list": [0],</text:p>
+            <text:p>
+              <text:span text:style-name="T2">"time_shift_list": [0],</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string" table:number-columns-spanned="1" table:number-rows-spanned="5">
+            <text:p>time_shift variation by step of 4</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>tb_tes_top_test_variant_debug06.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>"nb_pixel_by_frame": 34,</text:p>
+            <text:p>"nb_sample_by_pixel": 8,</text:p>
+            <text:p>"nb_frame_by_pulse": 2048,</text:p>
+            <text:p>"nb_pulse": 1,</text:p>
+            <text:p>"pulse_height_list": [58880],</text:p>
+            <text:p>"pixel_id_list": [0],</text:p>
+            <text:p>
+              <text:span text:style-name="T2">"time_shift_list": [3],</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:style-name="ce13"/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>tb_tes_top_test_variant_debug07.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>"nb_pixel_by_frame": 34,</text:p>
+            <text:p>"nb_sample_by_pixel": 8,</text:p>
+            <text:p>"nb_frame_by_pulse": 2048,</text:p>
+            <text:p>"nb_pulse": 1,</text:p>
+            <text:p>"pulse_height_list": [58880],</text:p>
+            <text:p>"pixel_id_list": [0],</text:p>
+            <text:p>
+              <text:span text:style-name="T2">"time_shift_list": [7],</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:style-name="ce13"/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>tb_tes_top_test_variant_debug08.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>"nb_pixel_by_frame": 34,</text:p>
+            <text:p>"nb_sample_by_pixel": 8,</text:p>
+            <text:p>"nb_frame_by_pulse": 2048,</text:p>
+            <text:p>"nb_pulse": 1,</text:p>
+            <text:p>"pulse_height_list": [58880],</text:p>
+            <text:p>"pixel_id_list": [0],</text:p>
+            <text:p>
+              <text:span text:style-name="T2">"time_shift_list": [11],</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:style-name="ce13"/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>tb_tes_top_test_variant_debug09.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>"nb_pixel_by_frame": 34,</text:p>
+            <text:p>"nb_sample_by_pixel": 8,</text:p>
+            <text:p>"nb_frame_by_pulse": 2048,</text:p>
+            <text:p>"nb_pulse": 1,</text:p>
+            <text:p>"pulse_height_list": [58880],</text:p>
+            <text:p>"pixel_id_list": [0],</text:p>
+            <text:p>
+              <text:span text:style-name="T2">"time_shift_list": [15],</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:style-name="ce13"/>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>tb_tes_top_test_variant_debug10.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce16" office:value-type="string" calcext:value-type="string">
+            <text:p>"nb_pixel_by_frame": 34,</text:p>
+            <text:p>"nb_sample_by_pixel": 8,</text:p>
+            <text:p>"nb_frame_by_pulse": 2048,</text:p>
+            <text:p>"nb_pulse": 1,</text:p>
+            <text:p>"pulse_height_list": [58880],</text:p>
+            <text:p>"pixel_id_list": [0],</text:p>
+            <text:p>
+              <text:span text:style-name="T3">"time_shift_list": [0],</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce19" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T6">sporadic data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Sporadic data input stream test (non nominal case)</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>tb_tes_top_test_variant_debug05.json</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>"nb_pixel_by_frame": 34,</text:p>
+            <text:p>"nb_sample_by_pixel": 8,</text:p>
+            <text:p>"nb_frame_by_pulse": 2048,</text:p>
+            <text:p>"nb_pulse": 1,</text:p>
+            <text:p>
+              <text:span text:style-name="T4">"pulse_height_list": [0],</text:span>
+            </text:p>
+            <text:p>"pixel_id_list": [0],</text:p>
+            <text:p>
+              <text:span text:style-name="T3">"time_shift_list": [0],</text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce20" office:value-type="string" calcext:value-type="string">
+            <text:p>
+              <text:span text:style-name="T1">Continuous data valid</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM1 check</text:span>
+            </text:p>
+            <text:p>
+              <text:span text:style-name="T1">Continuous RAM2 check </text:span>
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>pulse with a height of 0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1020"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1" table:number-rows-repeated="13">
+          <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell table:number-columns-repeated="1024"/>
@@ -414,11 +739,11 @@
 <file path=meta.xml><?xml version="1.0" encoding="utf-8"?>
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" office:version="1.3">
   <office:meta>
-    <dc:date>2023-05-30T10:32:18.892000000</dc:date>
-    <meta:editing-duration>PT1H33M42S</meta:editing-duration>
-    <meta:editing-cycles>8</meta:editing-cycles>
+    <dc:date>2023-06-02T13:28:14.010000000</dc:date>
+    <meta:editing-duration>PT1H52M36S</meta:editing-duration>
+    <meta:editing-cycles>10</meta:editing-cycles>
     <meta:generator>LibreOffice/7.2.4.1$Windows_X86_64 LibreOffice_project/27d75539669ac387bb498e35313b970b7fe9c4f9</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="36" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="72" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -429,15 +754,15 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">20041</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">33176</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">30578</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">55712</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Feuille1">
-              <config:config-item config:name="CursorPositionX" config:type="int">4</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">2</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">23</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
@@ -446,7 +771,7 @@
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">15</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -455,7 +780,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">Feuille1</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1855</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1599</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -490,6 +815,15 @@
       <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
       <config:config-item config:name="EmbedLatinScriptFonts" config:type="boolean">true</config:config-item>
       <config:config-item config:name="EmbedOnlyUsedFonts" config:type="boolean">false</config:config-item>
+      <config:config-item-map-indexed config:name="ForbiddenCharacters">
+        <config:config-item-map-entry>
+          <config:config-item config:name="Language" config:type="string">fr</config:config-item>
+          <config:config-item config:name="Country" config:type="string">FR</config:config-item>
+          <config:config-item config:name="Variant" config:type="string"/>
+          <config:config-item config:name="BeginLine" config:type="string"/>
+          <config:config-item config:name="EndLine" config:type="string"/>
+        </config:config-item-map-entry>
+      </config:config-item-map-indexed>
       <config:config-item config:name="GridColor" config:type="int">12632256</config:config-item>
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
@@ -658,9 +992,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2023-05-30">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2023-06-02">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="10:27:07.243000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="12:38:54.270000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
ci,tes: minor update rename tes_name: tb_tes_top_test_variant_debug05 into tb_tes_top_test_variant_debug11
</commit_message>
<xml_diff>
--- a/simu/conf/fpasim/tes/tes_top_test_list.xlsx
+++ b/simu/conf/fpasim/tes/tes_top_test_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fpasim-fw-hardware\simu\conf\fpasim\tes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726CFE7F-1484-491E-8A3B-9D919A1A458F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981D9234-96BD-4DD5-91EA-A49F127599B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
   <si>
     <t>test_name</t>
   </si>
@@ -1198,6 +1198,9 @@
       <t>"pixel_id_list": [0],
 "time_shift_list": [0],</t>
     </r>
+  </si>
+  <si>
+    <t>tb_tes_top_test_variant_debug11.json</t>
   </si>
 </sst>
 </file>
@@ -1637,8 +1640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1919,7 +1922,7 @@
     </row>
     <row r="23" spans="1:4" ht="102.75" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>54</v>

</xml_diff>